<commit_message>
finalised VO excel sheet for scarlet
</commit_message>
<xml_diff>
--- a/concept/sound/scarlet_sounds_sheet.xlsx
+++ b/concept/sound/scarlet_sounds_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
   <si>
     <t>Start</t>
   </si>
@@ -237,24 +237,12 @@
     <t>00:37.1</t>
   </si>
   <si>
-    <t>00:37.2</t>
-  </si>
-  <si>
     <t>00:38.6</t>
   </si>
   <si>
-    <t>00:38.8</t>
-  </si>
-  <si>
     <t>00:40.1</t>
   </si>
   <si>
-    <t>00:40.5</t>
-  </si>
-  <si>
-    <t>00:42.0</t>
-  </si>
-  <si>
     <t>00:50.5</t>
   </si>
   <si>
@@ -360,10 +348,100 @@
     <t>01:28.5</t>
   </si>
   <si>
-    <t>Als Female Fairy (Tammie) stirbt</t>
-  </si>
-  <si>
     <t>Als Male Fairy (Tommie) stirbt --&gt; Wechsel zu Phase 3 (parallel zu Tammies Weinanfall)</t>
+  </si>
+  <si>
+    <t>Scarlet_Kirche_M</t>
+  </si>
+  <si>
+    <t>00:18.6</t>
+  </si>
+  <si>
+    <t>00:19.6</t>
+  </si>
+  <si>
+    <t>00:20.16</t>
+  </si>
+  <si>
+    <t>00:20.9</t>
+  </si>
+  <si>
+    <t>00:21.4</t>
+  </si>
+  <si>
+    <t>00:22.3</t>
+  </si>
+  <si>
+    <t>00:23.1</t>
+  </si>
+  <si>
+    <t>00:25.6</t>
+  </si>
+  <si>
+    <t>01:01.8</t>
+  </si>
+  <si>
+    <t>01:10.2</t>
+  </si>
+  <si>
+    <t>Verbannung</t>
+  </si>
+  <si>
+    <t>01:13.7</t>
+  </si>
+  <si>
+    <t>01:15.1</t>
+  </si>
+  <si>
+    <t>01:18.3</t>
+  </si>
+  <si>
+    <t>01:19.6</t>
+  </si>
+  <si>
+    <t>01:20.1</t>
+  </si>
+  <si>
+    <t>01:20.6</t>
+  </si>
+  <si>
+    <t>01:39.1</t>
+  </si>
+  <si>
+    <t>01:45.1</t>
+  </si>
+  <si>
+    <t>DH / Angel besiegt (Humanity Destroyed Victory Screen / Death Defied Victory Screen)</t>
+  </si>
+  <si>
+    <t>01:15.9</t>
+  </si>
+  <si>
+    <t>01:17.3</t>
+  </si>
+  <si>
+    <t>Als Female Fairy (Tammie) stirbt (Light Annihilated Victory Screen)</t>
+  </si>
+  <si>
+    <t>01:23.4</t>
+  </si>
+  <si>
+    <t>01:24.1</t>
+  </si>
+  <si>
+    <t>01:24.4</t>
+  </si>
+  <si>
+    <t>01:25.1</t>
+  </si>
+  <si>
+    <t>Exploration</t>
+  </si>
+  <si>
+    <t>Notwendiger Dialog</t>
+  </si>
+  <si>
+    <t>Post Angel Cutscene</t>
   </si>
 </sst>
 </file>
@@ -419,8 +497,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -519,7 +631,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="127">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -566,6 +678,23 @@
     <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -612,6 +741,23 @@
     <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -941,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1207,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1436,7 +1582,7 @@
         <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
@@ -1453,7 +1599,7 @@
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1470,7 +1616,7 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1479,15 +1625,15 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1496,15 +1642,15 @@
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1518,10 +1664,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1530,35 +1676,12 @@
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="F42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1580,7 +1703,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
@@ -1597,10 +1720,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1617,7 +1740,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1631,10 +1754,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1648,7 +1771,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
         <v>59</v>
@@ -1660,15 +1783,15 @@
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1680,12 +1803,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1697,12 +1820,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1714,12 +1837,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1731,12 +1854,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1748,12 +1871,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1765,55 +1888,284 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="F61" t="s">
         <v>110</v>
       </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" t="s">
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" t="s">
-        <v>113</v>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" t="s">
+        <v>121</v>
+      </c>
+      <c r="G66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>122</v>
+      </c>
+      <c r="B67" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>127</v>
+      </c>
+      <c r="B71" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>136</v>
+      </c>
+      <c r="B74" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>128</v>
+      </c>
+      <c r="B76" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hopefully fixed sound specification sheet of scarlet
</commit_message>
<xml_diff>
--- a/concept/sound/scarlet_sounds_sheet.xlsx
+++ b/concept/sound/scarlet_sounds_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="137">
   <si>
     <t>Start</t>
   </si>
@@ -171,78 +171,30 @@
     <t>sämtliche Sounds nur für Pre-Werewolf Wald und Werewolf-Fight ausgelet</t>
   </si>
   <si>
-    <t>00:00.7</t>
-  </si>
-  <si>
-    <t>00:02.2</t>
-  </si>
-  <si>
-    <t>00:03.6</t>
-  </si>
-  <si>
     <t>&lt; 30% HP</t>
   </si>
   <si>
     <t>wir sollten das glaub ich weglassen</t>
   </si>
   <si>
-    <t>00:21.9</t>
-  </si>
-  <si>
     <t>00:22.6</t>
   </si>
   <si>
     <t>00:22.7</t>
   </si>
   <si>
-    <t>00:23.3</t>
-  </si>
-  <si>
     <t>00:23.6</t>
   </si>
   <si>
-    <t>00:24.1</t>
-  </si>
-  <si>
     <t>00:24.2</t>
   </si>
   <si>
-    <t>00:24.8</t>
-  </si>
-  <si>
-    <t>00:27.1</t>
-  </si>
-  <si>
-    <t>00:28.2</t>
-  </si>
-  <si>
-    <t>00:28.7</t>
-  </si>
-  <si>
-    <t>00:30.7</t>
-  </si>
-  <si>
-    <t>00:31.6</t>
-  </si>
-  <si>
-    <t>00:32.9</t>
-  </si>
-  <si>
-    <t>00:33.8</t>
-  </si>
-  <si>
     <t>00:35.8</t>
   </si>
   <si>
     <t>00:37.1</t>
   </si>
   <si>
-    <t>00:38.6</t>
-  </si>
-  <si>
-    <t>00:40.1</t>
-  </si>
-  <si>
     <t>00:50.5</t>
   </si>
   <si>
@@ -442,6 +394,42 @@
   </si>
   <si>
     <t>Post Angel Cutscene</t>
+  </si>
+  <si>
+    <t>00:22.0</t>
+  </si>
+  <si>
+    <t>00:24.0</t>
+  </si>
+  <si>
+    <t>00:24.7</t>
+  </si>
+  <si>
+    <t>00:28.8</t>
+  </si>
+  <si>
+    <t>00:29.6</t>
+  </si>
+  <si>
+    <t>00:29.9</t>
+  </si>
+  <si>
+    <t>00:30.5</t>
+  </si>
+  <si>
+    <t>00:30.8</t>
+  </si>
+  <si>
+    <t>00:37.3</t>
+  </si>
+  <si>
+    <t>00:38.5</t>
+  </si>
+  <si>
+    <t>00:40.5</t>
+  </si>
+  <si>
+    <t>00:41.9</t>
   </si>
 </sst>
 </file>
@@ -497,8 +485,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -631,7 +625,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="133">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -695,6 +689,9 @@
     <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -758,6 +755,9 @@
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1089,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1405,36 +1405,36 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>9</v>
+      <c r="A21" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
@@ -1443,15 +1443,15 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -1460,10 +1460,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -1476,11 +1476,11 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>55</v>
+      <c r="A25" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -1489,15 +1489,15 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
@@ -1511,10 +1511,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -1527,28 +1527,15 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -1557,15 +1544,15 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1578,45 +1565,22 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1625,15 +1589,15 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1642,15 +1606,15 @@
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1664,10 +1628,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1676,12 +1640,12 @@
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="F42" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1698,12 +1662,12 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
@@ -1720,10 +1684,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1740,7 +1704,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1754,10 +1718,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1771,10 +1735,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1788,10 +1752,10 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1805,10 +1769,10 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1822,10 +1786,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1839,10 +1803,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1856,10 +1820,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1873,10 +1837,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1890,10 +1854,10 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1902,15 +1866,15 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1919,15 +1883,15 @@
         <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1936,20 +1900,20 @@
         <v>6</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="F61" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B62" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1963,10 +1927,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1980,10 +1944,10 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1997,10 +1961,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -2009,35 +1973,35 @@
         <v>6</v>
       </c>
       <c r="E65" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="E66" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="G66" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -2051,10 +2015,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2068,10 +2032,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -2085,10 +2049,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2102,10 +2066,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2119,10 +2083,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
@@ -2131,15 +2095,15 @@
         <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -2148,15 +2112,15 @@
         <v>6</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
@@ -2165,7 +2129,7 @@
         <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more random git stuff
</commit_message>
<xml_diff>
--- a/concept/sound/scarlet_sounds_sheet.xlsx
+++ b/concept/sound/scarlet_sounds_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="137">
   <si>
     <t>Start</t>
   </si>
@@ -171,78 +171,30 @@
     <t>sämtliche Sounds nur für Pre-Werewolf Wald und Werewolf-Fight ausgelet</t>
   </si>
   <si>
-    <t>00:00.7</t>
-  </si>
-  <si>
-    <t>00:02.2</t>
-  </si>
-  <si>
-    <t>00:03.6</t>
-  </si>
-  <si>
     <t>&lt; 30% HP</t>
   </si>
   <si>
     <t>wir sollten das glaub ich weglassen</t>
   </si>
   <si>
-    <t>00:21.9</t>
-  </si>
-  <si>
     <t>00:22.6</t>
   </si>
   <si>
     <t>00:22.7</t>
   </si>
   <si>
-    <t>00:23.3</t>
-  </si>
-  <si>
     <t>00:23.6</t>
   </si>
   <si>
-    <t>00:24.1</t>
-  </si>
-  <si>
     <t>00:24.2</t>
   </si>
   <si>
-    <t>00:24.8</t>
-  </si>
-  <si>
-    <t>00:27.1</t>
-  </si>
-  <si>
-    <t>00:28.2</t>
-  </si>
-  <si>
-    <t>00:28.7</t>
-  </si>
-  <si>
-    <t>00:30.7</t>
-  </si>
-  <si>
-    <t>00:31.6</t>
-  </si>
-  <si>
-    <t>00:32.9</t>
-  </si>
-  <si>
-    <t>00:33.8</t>
-  </si>
-  <si>
     <t>00:35.8</t>
   </si>
   <si>
     <t>00:37.1</t>
   </si>
   <si>
-    <t>00:38.6</t>
-  </si>
-  <si>
-    <t>00:40.1</t>
-  </si>
-  <si>
     <t>00:50.5</t>
   </si>
   <si>
@@ -442,6 +394,42 @@
   </si>
   <si>
     <t>Post Angel Cutscene</t>
+  </si>
+  <si>
+    <t>00:22.0</t>
+  </si>
+  <si>
+    <t>00:24.0</t>
+  </si>
+  <si>
+    <t>00:24.7</t>
+  </si>
+  <si>
+    <t>00:28.8</t>
+  </si>
+  <si>
+    <t>00:29.6</t>
+  </si>
+  <si>
+    <t>00:29.9</t>
+  </si>
+  <si>
+    <t>00:30.5</t>
+  </si>
+  <si>
+    <t>00:30.8</t>
+  </si>
+  <si>
+    <t>00:37.3</t>
+  </si>
+  <si>
+    <t>00:38.5</t>
+  </si>
+  <si>
+    <t>00:40.5</t>
+  </si>
+  <si>
+    <t>00:41.9</t>
   </si>
 </sst>
 </file>
@@ -497,8 +485,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -631,7 +625,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="133">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -695,6 +689,9 @@
     <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -758,6 +755,9 @@
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1089,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1405,36 +1405,36 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>9</v>
+      <c r="A21" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
@@ -1443,15 +1443,15 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -1460,10 +1460,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -1476,11 +1476,11 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>55</v>
+      <c r="A25" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -1489,15 +1489,15 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
@@ -1511,10 +1511,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -1527,28 +1527,15 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -1557,15 +1544,15 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1578,45 +1565,22 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1625,15 +1589,15 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1642,15 +1606,15 @@
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1664,10 +1628,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1676,12 +1640,12 @@
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="F42" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1698,12 +1662,12 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
@@ -1720,10 +1684,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1740,7 +1704,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1754,10 +1718,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1771,10 +1735,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1788,10 +1752,10 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1805,10 +1769,10 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1822,10 +1786,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1839,10 +1803,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1856,10 +1820,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1873,10 +1837,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1890,10 +1854,10 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1902,15 +1866,15 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1919,15 +1883,15 @@
         <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1936,20 +1900,20 @@
         <v>6</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="F61" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B62" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1963,10 +1927,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1980,10 +1944,10 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1997,10 +1961,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -2009,35 +1973,35 @@
         <v>6</v>
       </c>
       <c r="E65" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="E66" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="G66" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -2051,10 +2015,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2068,10 +2032,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -2085,10 +2049,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2102,10 +2066,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2119,10 +2083,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
@@ -2131,15 +2095,15 @@
         <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -2148,15 +2112,15 @@
         <v>6</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
@@ -2165,7 +2129,7 @@
         <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>